<commit_message>
This is the actual code after experimenting with github.
</commit_message>
<xml_diff>
--- a/INPUT.xlsx
+++ b/INPUT.xlsx
@@ -14,17 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>asdvdv</t>
-  </si>
-  <si>
-    <t>sdv</t>
-  </si>
-  <si>
-    <t>33r</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -364,30 +354,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D7"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "This is the actual code after experimenting with github."
This reverts commit c7e616e859ce4df0d2fe8c96eaaea4861b82fe04.
</commit_message>
<xml_diff>
--- a/INPUT.xlsx
+++ b/INPUT.xlsx
@@ -14,7 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>asdvdv</t>
+  </si>
+  <si>
+    <t>sdv</t>
+  </si>
+  <si>
+    <t>33r</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -354,12 +364,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>